<commit_message>
Caught a data entry error in MR std dev- so I am re-running everything with MR in it. Also the error is HUGE for literature values for pups, so I am running it a few more times trying to figure out why its so big now.
Also graphing TEE
</commit_message>
<xml_diff>
--- a/Data/Stdev_MR_perc_time_withconversions.xlsx
+++ b/Data/Stdev_MR_perc_time_withconversions.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliaadelsheim/Documents/Thesis/otteR/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{640EA412-25F0-2B43-AD43-BA651B11580B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15956C03-5810-0746-A5B9-D987C6A2B323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="2000" windowWidth="26840" windowHeight="14920" xr2:uid="{28F3D7D0-05C4-724C-9111-31B53BFDE9B0}"/>
+    <workbookView xWindow="13940" yWindow="1180" windowWidth="26840" windowHeight="14920" xr2:uid="{28F3D7D0-05C4-724C-9111-31B53BFDE9B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -464,7 +464,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,18 +523,18 @@
         <v>0.28499999999999998</v>
       </c>
       <c r="F3" s="2">
-        <v>0.224</v>
+        <v>0.24399999999999999</v>
       </c>
       <c r="I3" s="1">
-        <v>0.93200000000000005</v>
+        <v>1.0129999999999999</v>
       </c>
       <c r="J3">
         <f>(I3/555.84)*1000</f>
-        <v>1.676741508347726</v>
+        <v>1.8224668969487621</v>
       </c>
       <c r="K3">
         <f>J3/7.48</f>
-        <v>0.22416330325504355</v>
+        <v>0.24364530707871149</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -563,18 +563,18 @@
         <v>0.223</v>
       </c>
       <c r="F5" s="2">
-        <v>0.85</v>
+        <v>0.85399999999999998</v>
       </c>
       <c r="I5" s="1">
-        <v>1.861</v>
+        <v>1.869</v>
       </c>
       <c r="J5">
         <f>(I5/292.68)*1000</f>
-        <v>6.3584802514691807</v>
+        <v>6.3858138581385813</v>
       </c>
       <c r="K5">
         <f t="shared" ref="K5:K7" si="0">J5/7.48</f>
-        <v>0.85006420474186906</v>
+        <v>0.85371843023243055</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -603,18 +603,18 @@
         <v>0.109</v>
       </c>
       <c r="F7" s="2">
-        <v>0.183</v>
+        <v>0.185</v>
       </c>
       <c r="I7" s="1">
-        <v>0.81169999999999998</v>
+        <v>0.81950000000000001</v>
       </c>
       <c r="J7">
         <f>(I7/591.48)*1000</f>
-        <v>1.3723202813281936</v>
+        <v>1.3855075404071142</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>0.18346527825243228</v>
+        <v>0.18522828080309012</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Found an error in my %time numbers for pups. Also updated juveniles and subsequently subadults. I fixed the values in the SA and then ran the all parameters literature variation SA analysis. Also redid graphs and output csv's just to be sure. I also reran the basic model to see how numbers changed. realllly small difference in #'s so nothing awful!
</commit_message>
<xml_diff>
--- a/Data/Stdev_MR_perc_time_withconversions.xlsx
+++ b/Data/Stdev_MR_perc_time_withconversions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliaadelsheim/Documents/Thesis/otteR/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15956C03-5810-0746-A5B9-D987C6A2B323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F121FEF-667C-4F46-9BC7-1A7F62D9BD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13940" yWindow="1180" windowWidth="26840" windowHeight="14920" xr2:uid="{28F3D7D0-05C4-724C-9111-31B53BFDE9B0}"/>
+    <workbookView xWindow="-22320" yWindow="1940" windowWidth="17580" windowHeight="14620" xr2:uid="{28F3D7D0-05C4-724C-9111-31B53BFDE9B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="22">
   <si>
     <t>Sex</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Unit Conversions for CSV</t>
+  </si>
+  <si>
+    <t>mlO2/kg*min</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,18 +526,18 @@
         <v>0.28499999999999998</v>
       </c>
       <c r="F3" s="2">
-        <v>0.24399999999999999</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="I3" s="1">
         <v>1.0129999999999999</v>
       </c>
       <c r="J3">
-        <f>(I3/555.84)*1000</f>
-        <v>1.8224668969487621</v>
+        <f>(I3/923.4)*1000</f>
+        <v>1.0970327052198396</v>
       </c>
       <c r="K3">
         <f>J3/7.48</f>
-        <v>0.24364530707871149</v>
+        <v>0.14666212636628873</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -603,18 +606,18 @@
         <v>0.109</v>
       </c>
       <c r="F7" s="2">
-        <v>0.185</v>
+        <v>0.49099999999999999</v>
       </c>
       <c r="I7" s="1">
         <v>0.81950000000000001</v>
       </c>
       <c r="J7">
-        <f>(I7/591.48)*1000</f>
-        <v>1.3855075404071142</v>
+        <f>(I7/223.2)*1000</f>
+        <v>3.6715949820788536</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>0.18522828080309012</v>
+        <v>0.49085494412818897</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -635,7 +638,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="2">
-        <v>0.152</v>
+        <v>0.153</v>
       </c>
       <c r="F9" s="2">
         <v>0.154</v>
@@ -715,7 +718,7 @@
         <v>14</v>
       </c>
       <c r="E13" s="2">
-        <v>9.1999999999999998E-2</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="F13" s="2">
         <v>0.129</v>
@@ -735,6 +738,9 @@
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
+      <c r="I14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -757,7 +763,11 @@
         <v>3.6063680000000001E-2</v>
       </c>
       <c r="I15" s="1">
-        <v>1.796</v>
+        <v>1.804</v>
+      </c>
+      <c r="J15">
+        <f>I15*20.08/1000</f>
+        <v>3.6224319999999997E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -769,7 +779,7 @@
       <c r="F16" s="2"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -786,14 +796,17 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="F17" s="2">
-        <f>6.244*20.08/1000</f>
-        <v>0.12537951999999999</v>
+        <v>0.126</v>
       </c>
       <c r="I17" s="1">
-        <v>6.2439999999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>6.2619999999999996</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ref="J17:J32" si="2">I17*20.08/1000</f>
+        <v>0.12574095999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -802,7 +815,7 @@
       <c r="F18" s="2"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -823,14 +836,22 @@
         <v>0.10795008</v>
       </c>
       <c r="I19" s="1">
-        <v>5.3760000000000003</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>5.3769999999999998</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>0.10797016</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -853,13 +874,17 @@
       <c r="I21" s="1">
         <v>2.552</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>5.1244159999999997E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -883,12 +908,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -912,11 +937,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -936,12 +961,19 @@
         <f>0.905*20.08/1000</f>
         <v>1.8172399999999998E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <v>0.90468231877835403</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="2"/>
+        <v>1.8166020961069347E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -961,12 +993,19 @@
         <f>2.951*20.08/1000</f>
         <v>5.9256079999999996E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I29">
+        <v>2.9506455721203002</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>5.9248963088175621E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -986,8 +1025,15 @@
         <f>1.683*20.08/1000</f>
         <v>3.3794640000000001E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I31">
+        <v>1.6833771689994701</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="2"/>
+        <v>3.3802213553509354E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
@@ -1005,7 +1051,7 @@
         <v>12</v>
       </c>
       <c r="E33" s="3">
-        <v>8.5999999999999993E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="F33" s="3">
         <v>7.6999999999999999E-2</v>
@@ -1053,10 +1099,10 @@
         <v>13</v>
       </c>
       <c r="E37" s="3">
-        <v>9.1999999999999998E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="F37" s="3">
-        <v>0.106</v>
+        <v>0.107</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1077,7 +1123,7 @@
         <v>12</v>
       </c>
       <c r="E39" s="2">
-        <v>0.152</v>
+        <v>0.153</v>
       </c>
       <c r="F39" s="2">
         <v>0.154</v>
@@ -1125,7 +1171,7 @@
         <v>14</v>
       </c>
       <c r="E43" s="2">
-        <v>9.1999999999999998E-2</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="F43" s="2">
         <v>0.129</v>
@@ -1152,7 +1198,7 @@
         <v>0.28499999999999998</v>
       </c>
       <c r="F45" s="2">
-        <v>0.224</v>
+        <v>0.14699999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1176,7 +1222,7 @@
         <v>0.223</v>
       </c>
       <c r="F47" s="2">
-        <v>0.85</v>
+        <v>0.85399999999999998</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1200,7 +1246,7 @@
         <v>0.109</v>
       </c>
       <c r="F49" s="2">
-        <v>0.183</v>
+        <v>0.49099999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>